<commit_message>
iEms data driven test ready, cinclude api-engine test
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD011BBA-C9DA-4ED7-BA17-07995A5C4714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2097210-80EA-4F26-9D65-2C2745EBE0BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>[SensorData][][][updateTime dsc][1,15]</t>
   </si>
   <si>
-    <t>[SensorData][][{_and: [{updateTime: {_gt: "2020-09-27 04:00:00"}},{updateTime: {_lt: "2020-10-01 03:00:00"}}]}]</t>
-  </si>
-  <si>
     <t>query</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>{SensorData(cond:"{Siid: {_invalid: 999999}}")  {Siid type value}}</t>
+  </si>
+  <si>
+    <t>[SensorData][][{_and: [{updateTime: {_gt: "2020-11-27 04:00:00"}},{updateTime: {_lt: "2020-12-01 03:00:00"}}]}]</t>
   </si>
 </sst>
 </file>
@@ -517,9 +517,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -613,7 +613,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
@@ -783,7 +783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -803,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -817,13 +817,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="D2" s="3">
         <v>200</v>
@@ -837,13 +837,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="D3" s="3">
         <v>200</v>
@@ -852,18 +852,18 @@
         <v>101301</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="D4" s="3">
         <v>200</v>
@@ -877,13 +877,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D5" s="3">
         <v>200</v>
@@ -897,13 +897,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3">
         <v>200</v>
@@ -912,7 +912,7 @@
         <v>101302</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve iEMS test, remove run time error reported by Allure
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2097210-80EA-4F26-9D65-2C2745EBE0BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6172F5-6B2C-4DD5-B6B4-59CCFAA12A51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>description</t>
   </si>
@@ -88,12 +88,6 @@
     <t>iems-api-engine-restful-test-7</t>
   </si>
   <si>
-    <t>[SensorData][type,Siid][{Siid: {_in: [34268,35768,33432,33173,36483]}}][][]</t>
-  </si>
-  <si>
-    <t>[SensorData][type,Siid][{Siid: {_nin: [34268,35768,33432,33173,36483]}}][][]</t>
-  </si>
-  <si>
     <t>iems-api-engine-restful-test-8</t>
   </si>
   <si>
@@ -158,6 +152,24 @@
   </si>
   <si>
     <t>[SensorData][][{_and: [{updateTime: {_gt: "2020-11-27 04:00:00"}},{updateTime: {_lt: "2020-12-01 03:00:00"}}]}]</t>
+  </si>
+  <si>
+    <t>iems-api-engine-graphql-test-6</t>
+  </si>
+  <si>
+    <t>{SensorData(cond:"{Siid: {_in: [5040, 5045, 34155]}}") {Siid type value}}</t>
+  </si>
+  <si>
+    <t>iems-api-engine-graphql-test-7</t>
+  </si>
+  <si>
+    <t>{SensorData(cond:"{Siid: {_nin: [5040, 5045, 34155]}}") {Siid type value}}</t>
+  </si>
+  <si>
+    <t>[SensorData][type,Siid][{Siid: {_in: [5040, 5045, 34155]}}][][]</t>
+  </si>
+  <si>
+    <t>[SensorData][type,Siid][{Siid: {_nin: [5040, 5045, 34155]}}][][]</t>
   </si>
 </sst>
 </file>
@@ -519,7 +531,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -613,7 +625,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
@@ -637,7 +649,7 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>13</v>
@@ -685,7 +697,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>13</v>
@@ -702,14 +714,14 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>13</v>
@@ -726,7 +738,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
@@ -750,14 +762,14 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>13</v>
@@ -781,10 +793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -803,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -817,13 +829,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3">
         <v>200</v>
@@ -837,13 +849,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D3" s="3">
         <v>200</v>
@@ -852,18 +864,18 @@
         <v>101301</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3">
         <v>200</v>
@@ -877,13 +889,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>200</v>
@@ -897,13 +909,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="D6" s="3">
         <v>200</v>
@@ -912,7 +924,47 @@
         <v>101302</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="3">
+        <v>200</v>
+      </c>
+      <c r="E7" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="3">
+        <v>200</v>
+      </c>
+      <c r="E8" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add case for iems configuration api
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FF4CFE-8C8B-44D4-809E-3B67A0183B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FB5C18-ADC9-4E66-A69B-E3A45A728C15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="78">
   <si>
     <t>description</t>
   </si>
@@ -192,6 +192,75 @@
   <si>
     <t xml:space="preserve">{Analog(cond:"{Siid: {_invalid: 999999}}") {Analog_id Siid aliasName description deviceId}} 
     </t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_TRAINCONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_TRAINRESULT</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_PREDICTCONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_OPTIMALIZERESULT</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_OPTIMALIZECONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_SIMULATION</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_TOPOLOGY</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_OPTIMIZE_TARGET_TYPE</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_DASHBOARDCONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_METADATA</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_SECTIONALIZEDLINEARIZATION</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_PREDICTRESULT</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_TRAINCONFIG(cond:"",order:"id DESC") { createTime id optimize_target_type_id simu_id train_cfg_ANN_YN train_cfg_LR_YN train_cfg_RFR_YN train_cfg_SVR_YN train_cfg_SmpEndTime train_cfg_SmpStTime train_cfg_Tree_YN train_cfg_aDa_YN train_cfg_obj_PT train_cfg_obligate1 train_cfg_obligate2 train_cfg_obligate3 train_cfg_obligate4 train_cfg_obligate5 train_cfg_obligate6 train_cfg_predict train_cfg_sample_PT train_cfg_time train_cfg_timetrg_YN}}</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_TRAINRESULT(cond:"",order:"id ASC") { variables train_result_obligate4 train_result_obligate5 train_result_obligate2 train_result_obligate3 optimize_target_type_id simu_id train_result_obligate1 config_id train_result_obligate6 id runid }}</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_PREDICTCONFIG(cond:"",order:"id ASC") { predict_train_model createTime predict_train_obj_wgt_defval predict_cfg_obligate6 predict_cfg_obligate5 predict_cfg_obligate4 predict_cfg_obligate3 predict_cfg_obligate2 predict_cfg_obligate1 optimize_target_type_id simu_id predict_cfg_period predict_cfg_day predict_cfg_time id } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_PREDICTRESULT(cond:"",order:"config_id ASC") { Predict_result_time Predict_result_aDa Predict_result_ANN optimize_target_type_id Predict_result_SP5 Predict_result_Tree Predict_result_LR Predict_result_SVR runid id createTime variables predict_train_obj_wgt_defval Predict_result_obligate2 Predict_result_obligate1 Predict_result_RFR Predict_result_obligate6 simu_id Predict_result_obligate5 Predict_result_obligate4 Predict_result_obligate3 config_id Predict_result_AVG } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_OPTIMALIZECONFIG(cond:"",order:"id ASC") { isActive optimize_target_type_id optimalizeType opt_cfg_opt_starttime id opt_cfg_user_def opt_pred_model opt_cfg_obligate3 rollTasksId opt_cfg_obligate2 opt_cfg_obligate5 createTime opt_cfg_obligate4 opt_cfg_obligate6 opt_cfg_emi_frac opt_name dash_cfg_id simu_id opt_cfg_opt_day opt_cfg_opt_frequency isRTCOP opt_cfg_cost_frac opt_methods rollType opt_cfg_obligate1 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_SIMULATION(cond:"",order:"id ASC") { updatatime historymap chartsetting createtime rtcountmap hiscountmap isTraining obligate1 obligate2 channels defcountmap user_id ispredict name id obligate5 obligate6 treefile obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_TOPOLOGY(cond:"",order:"id ASC") { create_time topo_name simu_id obligate1 obligate2 topo_xml update_time update_user parent_id id obligate5 obligate6 obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_OPTIMIZE_TARGET_TYPE(cond:"",order:"id ASC") { obligate1 obligate2 optimize_topo_selection optimize_type optimize_name id obligate5 optimize_data_type obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_DASHBOARDCONFIG(cond:"",order:"id ASC") { dashparam name id simu_id optimize_target_type_id } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_METADATA(cond:"",order:"id ASC") { obligate1 obligate2 name id obligate5 params category obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_SECTIONALIZEDLINEARIZATION(cond:"",order:"id ASC") { tensor_index_counts target obligate1 obligate2 device_name model_name param id obligate5 obligate3 obligate4 tensor_data } }</t>
   </si>
 </sst>
 </file>
@@ -554,20 +623,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" style="1"/>
-    <col min="4" max="4" width="36.6328125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="12.6328125" style="1"/>
+    <col min="1" max="2" width="30.61328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.61328125" style="1"/>
+    <col min="4" max="4" width="36.61328125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="12.61328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -593,7 +662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -617,7 +686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -641,7 +710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -665,7 +734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -689,7 +758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -713,7 +782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -737,7 +806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -761,7 +830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -785,7 +854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -818,21 +887,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.6328125" style="6" customWidth="1"/>
-    <col min="4" max="6" width="12.6328125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="41.69140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.61328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.61328125" style="6" customWidth="1"/>
+    <col min="4" max="6" width="12.61328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.84375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -852,7 +922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -872,7 +942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -892,7 +962,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -912,7 +982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -932,7 +1002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
@@ -952,7 +1022,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
@@ -972,7 +1042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
@@ -992,7 +1062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>49</v>
       </c>
@@ -1012,7 +1082,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
@@ -1032,7 +1102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -1050,6 +1120,246 @@
       </c>
       <c r="F11" s="3" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="3">
+        <v>200</v>
+      </c>
+      <c r="E12" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="3">
+        <v>200</v>
+      </c>
+      <c r="E13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="3">
+        <v>200</v>
+      </c>
+      <c r="E14" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="3">
+        <v>200</v>
+      </c>
+      <c r="E15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="3">
+        <v>200</v>
+      </c>
+      <c r="E16" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="3">
+        <v>200</v>
+      </c>
+      <c r="E17" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="3">
+        <v>200</v>
+      </c>
+      <c r="E18" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="3">
+        <v>200</v>
+      </c>
+      <c r="E19" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="3">
+        <v>200</v>
+      </c>
+      <c r="E20" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="3">
+        <v>200</v>
+      </c>
+      <c r="E21" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="3">
+        <v>200</v>
+      </c>
+      <c r="E22" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="3">
+        <v>200</v>
+      </c>
+      <c r="E23" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge with dev branch
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FF4CFE-8C8B-44D4-809E-3B67A0183B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FB5C18-ADC9-4E66-A69B-E3A45A728C15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="78">
   <si>
     <t>description</t>
   </si>
@@ -192,6 +192,75 @@
   <si>
     <t xml:space="preserve">{Analog(cond:"{Siid: {_invalid: 999999}}") {Analog_id Siid aliasName description deviceId}} 
     </t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_TRAINCONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_TRAINRESULT</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_PREDICTCONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_OPTIMALIZERESULT</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_OPTIMALIZECONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_SIMULATION</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_TOPOLOGY</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_OPTIMIZE_TARGET_TYPE</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_DASHBOARDCONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_METADATA</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_SECTIONALIZEDLINEARIZATION</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_PREDICTRESULT</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_TRAINCONFIG(cond:"",order:"id DESC") { createTime id optimize_target_type_id simu_id train_cfg_ANN_YN train_cfg_LR_YN train_cfg_RFR_YN train_cfg_SVR_YN train_cfg_SmpEndTime train_cfg_SmpStTime train_cfg_Tree_YN train_cfg_aDa_YN train_cfg_obj_PT train_cfg_obligate1 train_cfg_obligate2 train_cfg_obligate3 train_cfg_obligate4 train_cfg_obligate5 train_cfg_obligate6 train_cfg_predict train_cfg_sample_PT train_cfg_time train_cfg_timetrg_YN}}</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_TRAINRESULT(cond:"",order:"id ASC") { variables train_result_obligate4 train_result_obligate5 train_result_obligate2 train_result_obligate3 optimize_target_type_id simu_id train_result_obligate1 config_id train_result_obligate6 id runid }}</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_PREDICTCONFIG(cond:"",order:"id ASC") { predict_train_model createTime predict_train_obj_wgt_defval predict_cfg_obligate6 predict_cfg_obligate5 predict_cfg_obligate4 predict_cfg_obligate3 predict_cfg_obligate2 predict_cfg_obligate1 optimize_target_type_id simu_id predict_cfg_period predict_cfg_day predict_cfg_time id } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_PREDICTRESULT(cond:"",order:"config_id ASC") { Predict_result_time Predict_result_aDa Predict_result_ANN optimize_target_type_id Predict_result_SP5 Predict_result_Tree Predict_result_LR Predict_result_SVR runid id createTime variables predict_train_obj_wgt_defval Predict_result_obligate2 Predict_result_obligate1 Predict_result_RFR Predict_result_obligate6 simu_id Predict_result_obligate5 Predict_result_obligate4 Predict_result_obligate3 config_id Predict_result_AVG } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_OPTIMALIZECONFIG(cond:"",order:"id ASC") { isActive optimize_target_type_id optimalizeType opt_cfg_opt_starttime id opt_cfg_user_def opt_pred_model opt_cfg_obligate3 rollTasksId opt_cfg_obligate2 opt_cfg_obligate5 createTime opt_cfg_obligate4 opt_cfg_obligate6 opt_cfg_emi_frac opt_name dash_cfg_id simu_id opt_cfg_opt_day opt_cfg_opt_frequency isRTCOP opt_cfg_cost_frac opt_methods rollType opt_cfg_obligate1 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_SIMULATION(cond:"",order:"id ASC") { updatatime historymap chartsetting createtime rtcountmap hiscountmap isTraining obligate1 obligate2 channels defcountmap user_id ispredict name id obligate5 obligate6 treefile obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_TOPOLOGY(cond:"",order:"id ASC") { create_time topo_name simu_id obligate1 obligate2 topo_xml update_time update_user parent_id id obligate5 obligate6 obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_OPTIMIZE_TARGET_TYPE(cond:"",order:"id ASC") { obligate1 obligate2 optimize_topo_selection optimize_type optimize_name id obligate5 optimize_data_type obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_DASHBOARDCONFIG(cond:"",order:"id ASC") { dashparam name id simu_id optimize_target_type_id } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_METADATA(cond:"",order:"id ASC") { obligate1 obligate2 name id obligate5 params category obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_SECTIONALIZEDLINEARIZATION(cond:"",order:"id ASC") { tensor_index_counts target obligate1 obligate2 device_name model_name param id obligate5 obligate3 obligate4 tensor_data } }</t>
   </si>
 </sst>
 </file>
@@ -554,20 +623,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" style="1"/>
-    <col min="4" max="4" width="36.6328125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="12.6328125" style="1"/>
+    <col min="1" max="2" width="30.61328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.61328125" style="1"/>
+    <col min="4" max="4" width="36.61328125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="12.61328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -593,7 +662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -617,7 +686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -641,7 +710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -665,7 +734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -689,7 +758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -713,7 +782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -737,7 +806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -761,7 +830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -785,7 +854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -818,21 +887,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.6328125" style="6" customWidth="1"/>
-    <col min="4" max="6" width="12.6328125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="41.69140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.61328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.61328125" style="6" customWidth="1"/>
+    <col min="4" max="6" width="12.61328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.84375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -852,7 +922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -872,7 +942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -892,7 +962,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -912,7 +982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -932,7 +1002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
@@ -952,7 +1022,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
@@ -972,7 +1042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
@@ -992,7 +1062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>49</v>
       </c>
@@ -1012,7 +1082,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
@@ -1032,7 +1102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -1050,6 +1120,246 @@
       </c>
       <c r="F11" s="3" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="3">
+        <v>200</v>
+      </c>
+      <c r="E12" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="3">
+        <v>200</v>
+      </c>
+      <c r="E13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="3">
+        <v>200</v>
+      </c>
+      <c r="E14" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="3">
+        <v>200</v>
+      </c>
+      <c r="E15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="3">
+        <v>200</v>
+      </c>
+      <c r="E16" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="3">
+        <v>200</v>
+      </c>
+      <c r="E17" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="3">
+        <v>200</v>
+      </c>
+      <c r="E18" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="3">
+        <v>200</v>
+      </c>
+      <c r="E19" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="3">
+        <v>200</v>
+      </c>
+      <c r="E20" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="3">
+        <v>200</v>
+      </c>
+      <c r="E21" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="3">
+        <v>200</v>
+      </c>
+      <c r="E22" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="3">
+        <v>200</v>
+      </c>
+      <c r="E23" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test cases for RestfulAsDataSourcesEnhanceTests/queryPostgresqlData
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FB5C18-ADC9-4E66-A69B-E3A45A728C15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDCDF77-DD46-4837-A6D9-E79CEA830A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
     <sheet name="getDataGraphQL" sheetId="3" r:id="rId2"/>
+    <sheet name="queryPostgresqlData" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="133">
   <si>
     <t>description</t>
   </si>
@@ -261,13 +262,787 @@
   </si>
   <si>
     <t>{CIMSOURCE_SECTIONALIZEDLINEARIZATION(cond:"",order:"id ASC") { tensor_index_counts target obligate1 obligate2 device_name model_name param id obligate5 obligate3 obligate4 tensor_data } }</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-1</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+Building-&gt;Floor-&gt;Room
+楼宇信息 楼层信息 区域信息</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>{
+  Building(cond:"", authInfo:"", order:"")
+  {
+    _isPartOf
+    sourceId
+    description
+    type
+    id
+    name
+    hasPart_Floor(cond:"", authInfo:"", order:"")
+    {
+      _isPartOf
+      sourceId
+      description
+      type
+      id
+      name
+      hasPart_Room(cond:"", authInfo:"", order:"")
+      {
+        _isPartOf
+        sourceId
+        description
+        type
+        id
+        name
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-2</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+Building-&gt;Floor
+根据指定楼宇获取楼层列表</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-3</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+Floor-&gt;Room
+根据指定楼层获取空间列表</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-4</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">good request, data retrieved
+Floor-&gt;Equipment
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Floor-&gt;Room-&gt;EquipmentLocation-&gt;Equipment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+根据楼层获得所有设备信息</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"", authInfo:"", order:"")
+  {
+    _isPartOf
+    sourceId
+    description
+    type
+    id
+    name
+    hasPart_Room(cond:"", authInfo:"", order:"")
+    {
+      _isPartOf
+      sourceId
+      description
+      type
+      id
+      name
+      isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
+      {
+        location
+        id
+        equipment
+        isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
+        {
+          _isPartOf
+          sourceId
+          description
+          type
+          id
+          name
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">good request, data retrieved
+Floor-&gt;Equipment
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Floor-&gt;Room-&gt;EquipmentLocation-&gt;Equipment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+根据指定楼层获取设备列表</t>
+    </r>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-6</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">good request, data retrieved
+Room-&gt;Equipment
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Room-&gt;EquipmentLocation-&gt;Equipment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+根据空间id查询设备列表</t>
+    </r>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-7</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">good request, data retrieved
+Floor-&gt;Equipment
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Floor-&gt;Room-&gt;EquipmentLocation-&gt;Equipment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+模糊查询设备(需要添加condition)</t>
+    </r>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-8</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+查询Mode Sensor 及mode option（涵盖模式枚举信息）</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-9</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+获取会议室当前模式及各需求点位信息</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-10</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+获取会议室模式sensor及模式option</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-11</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">good request, data retrieved
+Room-&gt;Equipment-&gt;Sensor-&gt;Mode_Sensor-&gt;Mode_Option
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Room-&gt;EquipmentLocation-&gt;Equipment-&gt;Point-&gt;Sensor-&gt;Mode_Sensor-&gt;Mode_Option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+根据device id获取mode sensor</t>
+    </r>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-12</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+获取当前会议室/工位占用传感器数据</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-13</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+获取当前会议室/工位占用传感器数据 增加时间条件</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-14</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+获取楼层占用传感器使用情况数据</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-15</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-16</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-17</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">good request, data retrieved
+Floor-&gt;Equipment-&gt;Room_Controller-&gt;Temperature_Sensor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Floor-&gt;Room-&gt;EquipmentLocation-&gt;Equipment?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+查询室内温度</t>
+    </r>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-18</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-19</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-20</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">good request, data retrieved
+Floor-&gt;Sensor-&gt;PM25_Sensor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Floor-&gt;PointLocation-&gt;PM25_Sensor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+获取PM2.5浓度</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  Building(cond:"{id:{_eq:\"d68ea3cf6be94281a785338afaa9205d\"}}", authInfo:"", order:"")
+  {
+    _isPartOf
+    sourceId
+    description
+    type
+    id
+    name
+    hasPart_Floor(cond:"", authInfo:"", order:"")
+    {
+      _isPartOf
+      sourceId
+      description
+      type
+      id
+      name
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"{id:{_eq:\"e8130762852a48cfafb5546e4e8a7413\"}}", authInfo:"", order:"")
+  {
+    _isPartOf
+    sourceId
+    description
+    type
+    id
+    name
+    hasPart_Room(cond:"", authInfo:"", order:"")
+    {
+      _isPartOf
+      sourceId
+      description
+      type
+      id
+      name
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"{id:{_eq:\"e8130762852a48cfafb5546e4e8a7413\"}}", authInfo:"", order:"")
+  {
+    _isPartOf
+    sourceId
+    description
+    type
+    id
+    name
+    hasPart_Room(cond:"", authInfo:"", order:"")
+    {
+      _isPartOf
+      sourceId
+      description
+      type
+      id
+      name
+      isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
+      {
+        location
+        id
+        equipment
+        isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
+        {
+          _isPartOf
+          sourceId
+          description
+          type
+          id
+          name
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Room(cond:"{id:{_eq:\"96042959aad644d5b993d1373461bdd0\"}}", authInfo:"", order:"")
+  {
+    _isPartOf
+    sourceId
+    description
+    type
+    id
+    name
+    isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
+    {
+      location
+      id
+      equipment
+      isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
+      {
+        _isPartOf
+        sourceId
+        description
+        type
+        id
+        name
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"", authInfo:"", order:"")
+  {
+    _isPartOf
+    sourceId
+    description
+    type
+    id
+    name
+    hasPart_Room(cond:"", authInfo:"", order:"")
+    {
+      _isPartOf
+      sourceId
+      description
+      type
+      id
+      name
+      isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
+      {
+        location
+        id
+        equipment
+        isEquipmentLocationOf_Equipment(cond:"{name:{_like:\"SS_Mock_B1.F2.RM13.CT2%\"}}", authInfo:"", order:"")
+        {
+          _isPartOf
+          sourceId
+          description
+          type
+          id
+          name
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"", authInfo:"", order:"")
+  {
+    sourceId
+    name
+    description
+    id
+    _isPartOf
+    type
+    subClassOf_Location(cond:"", authInfo:"", order:"")
+    {
+      sourceId
+      name
+      description
+      id
+      _isPartOf
+      type
+      isLocationOf_PointLocation(cond:"", authInfo:"", order:"")
+      {
+        id
+        location
+        point
+        isPointLocationOf_Power_Sensor(cond:"", authInfo:"", order:"")
+        {
+          sourceId
+          sourceSystem
+          name
+          description
+          id
+          _isPointOf
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">good request, data retrieved
+Floor-&gt;Sensor-&gt;Power_Sensor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Floor-&gt;Location-&gt;PointLocation-&gt;Power_Sensor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+获取能耗值</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">good request, data retrieved
+Floor-&gt;Sensor-&gt;Temperature_Sensor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Floorr-&gt;Location-&gt;PointLocation-&gt;Temperature_Sensor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+获取温度值</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"", authInfo:"", order:"")
+  {
+    sourceId
+    name
+    description
+    id
+    _isPartOf
+    type
+    subClassOf_Location(cond:"", authInfo:"", order:"")
+    {
+      sourceId
+      name
+      description
+      id
+      _isPartOf
+      type
+      isLocationOf_PointLocation(cond:"", authInfo:"", order:"")
+      {
+        id
+        location
+        point
+        isPointLocationOf_Temperature_Sensor(cond:"", authInfo:"", order:"")
+        {
+          sourceId
+          sourceSystem
+          name
+          description
+          id
+          _isPointOf
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">good request, data retrieved
+Floor-&gt;Sensor-&gt;Humidity_Sensor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Floor-&gt;Location-&gt;PointLocation-&gt;Humidity_Sensor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>获取湿度</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">good request, data retrieved
+Floor-&gt;Sensor-&gt;CO2_Sensor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Floor-&gt;Location-&gt;PointLocation-&gt;CO2_Sensor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+获取CO2浓度</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"", authInfo:"", order:"")
+  {
+    sourceId
+    name
+    description
+    id
+    _isPartOf
+    type
+    subClassOf_Location(cond:"", authInfo:"", order:"")
+    {
+      sourceId
+      name
+      description
+      id
+      _isPartOf
+      type
+      isLocationOf_PointLocation(cond:"", authInfo:"", order:"")
+      {
+        id
+        location
+        point
+        isPointLocationOf_Humidity_Sensor(cond:"", authInfo:"", order:"")
+        {
+          sourceId
+          sourceSystem
+          name
+          description
+          id
+          _isPointOf
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"", authInfo:"", order:"")
+  {
+    sourceId
+    name
+    description
+    id
+    _isPartOf
+    type
+    subClassOf_Location(cond:"", authInfo:"", order:"")
+    {
+      sourceId
+      name
+      description
+      id
+      _isPartOf
+      type
+      isLocationOf_PointLocation(cond:"", authInfo:"", order:"")
+      {
+        id
+        location
+        point
+        isPointLocationOf_CO2_Sensor(cond:"", authInfo:"", order:"")
+        {
+          sourceId
+          sourceSystem
+          name
+          description
+          id
+          _isPointOf
+          type
+        }
+      }
+    }
+  }
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +1059,19 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -330,7 +1118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -340,6 +1128,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,20 +1426,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.61328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.61328125" style="1"/>
-    <col min="4" max="4" width="36.61328125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="12.61328125" style="1"/>
+    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="1"/>
+    <col min="4" max="4" width="36.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -662,7 +1465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -686,7 +1489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -710,7 +1513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -734,7 +1537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -758,7 +1561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -782,7 +1585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -806,7 +1609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -830,7 +1633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -854,7 +1657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -889,20 +1692,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.69140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.61328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.61328125" style="6" customWidth="1"/>
-    <col min="4" max="6" width="12.61328125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.84375" style="1"/>
+    <col min="1" max="1" width="41.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.6640625" style="6" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -922,7 +1725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -942,7 +1745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -962,7 +1765,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -982,7 +1785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -1002,7 +1805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
@@ -1022,7 +1825,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
@@ -1042,7 +1845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
@@ -1062,7 +1865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>49</v>
       </c>
@@ -1082,7 +1885,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
@@ -1102,7 +1905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -1122,7 +1925,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -1142,7 +1945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
@@ -1162,7 +1965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
@@ -1182,7 +1985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
@@ -1202,7 +2005,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
@@ -1222,7 +2025,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1242,7 +2045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
@@ -1262,7 +2065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
@@ -1282,7 +2085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
@@ -1302,7 +2105,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
@@ -1322,7 +2125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
@@ -1342,7 +2145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
@@ -1367,4 +2170,469 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95BF81D-F35A-4340-837F-62C66C86E4D8}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="12">
+        <v>200</v>
+      </c>
+      <c r="F2" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="12">
+        <v>200</v>
+      </c>
+      <c r="F3" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="12">
+        <v>200</v>
+      </c>
+      <c r="F4" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="12">
+        <v>200</v>
+      </c>
+      <c r="F5" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="12">
+        <v>200</v>
+      </c>
+      <c r="F6" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="12">
+        <v>200</v>
+      </c>
+      <c r="F7" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="12">
+        <v>200</v>
+      </c>
+      <c r="F8" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="12">
+        <v>200</v>
+      </c>
+      <c r="F9" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="12">
+        <v>200</v>
+      </c>
+      <c r="F10" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="12">
+        <v>200</v>
+      </c>
+      <c r="F11" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test cases for SDL-8011/SDL-8224
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69547F5B-F779-43F5-8460-43ABE2F682CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FC0018-5F3C-4E80-A867-763C518707DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="queryPostgresqlData" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">queryPostgresqlData!$A$1:$H$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">queryPostgresqlData!$A$1:$G$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="252">
   <si>
     <t>description</t>
   </si>
@@ -280,37 +280,6 @@
   </si>
   <si>
     <t>Building</t>
-  </si>
-  <si>
-    <t>{
-  Building(cond:"", authInfo:"", order:"")
-  {
-    _isPartOf
-    sourceId
-    description
-    type
-    id
-    name
-    hasPart_Floor(cond:"", authInfo:"", order:"")
-    {
-      _isPartOf
-      sourceId
-      description
-      type
-      id
-      name
-      hasPart_Room(cond:"", authInfo:"", order:"")
-      {
-        _isPartOf
-        sourceId
-        description
-        type
-        id
-        name
-      }
-    }
-  }
-}</t>
   </si>
   <si>
     <t>databrain-queryPostgresqlData-test-2</t>
@@ -362,43 +331,6 @@
     </r>
   </si>
   <si>
-    <t>{
-  Floor(cond:"", authInfo:"", order:"")
-  {
-    _isPartOf
-    sourceId
-    description
-    type
-    id
-    name
-    hasPart_Room(cond:"", authInfo:"", order:"")
-    {
-      _isPartOf
-      sourceId
-      description
-      type
-      id
-      name
-      isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
-      {
-        location
-        id
-        equipment
-        isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
-        {
-          _isPartOf
-          sourceId
-          description
-          type
-          id
-          name
-        }
-      }
-    }
-  }
-}</t>
-  </si>
-  <si>
     <t>databrain-queryPostgresqlData-test-5</t>
   </si>
   <si>
@@ -634,152 +566,6 @@
       <t xml:space="preserve">
 获取PM2.5浓度</t>
     </r>
-  </si>
-  <si>
-    <t>{
-  Building(cond:"{id:{_eq:\"d68ea3cf6be94281a785338afaa9205d\"}}", authInfo:"", order:"")
-  {
-    _isPartOf
-    sourceId
-    description
-    type
-    id
-    name
-    hasPart_Floor(cond:"", authInfo:"", order:"")
-    {
-      _isPartOf
-      sourceId
-      description
-      type
-      id
-      name
-    }
-  }
-}</t>
-  </si>
-  <si>
-    <t>{
-  Floor(cond:"{id:{_eq:\"e8130762852a48cfafb5546e4e8a7413\"}}", authInfo:"", order:"")
-  {
-    _isPartOf
-    sourceId
-    description
-    type
-    id
-    name
-    hasPart_Room(cond:"", authInfo:"", order:"")
-    {
-      _isPartOf
-      sourceId
-      description
-      type
-      id
-      name
-    }
-  }
-}</t>
-  </si>
-  <si>
-    <t>{
-  Floor(cond:"{id:{_eq:\"e8130762852a48cfafb5546e4e8a7413\"}}", authInfo:"", order:"")
-  {
-    _isPartOf
-    sourceId
-    description
-    type
-    id
-    name
-    hasPart_Room(cond:"", authInfo:"", order:"")
-    {
-      _isPartOf
-      sourceId
-      description
-      type
-      id
-      name
-      isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
-      {
-        location
-        id
-        equipment
-        isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
-        {
-          _isPartOf
-          sourceId
-          description
-          type
-          id
-          name
-        }
-      }
-    }
-  }
-}</t>
-  </si>
-  <si>
-    <t>{
-  Room(cond:"{id:{_eq:\"96042959aad644d5b993d1373461bdd0\"}}", authInfo:"", order:"")
-  {
-    _isPartOf
-    sourceId
-    description
-    type
-    id
-    name
-    isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
-    {
-      location
-      id
-      equipment
-      isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
-      {
-        _isPartOf
-        sourceId
-        description
-        type
-        id
-        name
-      }
-    }
-  }
-}</t>
-  </si>
-  <si>
-    <t>{
-  Floor(cond:"", authInfo:"", order:"")
-  {
-    _isPartOf
-    sourceId
-    description
-    type
-    id
-    name
-    hasPart_Room(cond:"", authInfo:"", order:"")
-    {
-      _isPartOf
-      sourceId
-      description
-      type
-      id
-      name
-      isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
-      {
-        location
-        id
-        equipment
-        isEquipmentLocationOf_Equipment(cond:"{name:{_like:\"SS_Mock_B1.F2.RM13.CT2%\"}}", authInfo:"", order:"")
-        {
-          _isPartOf
-          sourceId
-          description
-          type
-          id
-          name
-        }
-      }
-    }
-  }
-}</t>
   </si>
   <si>
     <t>{
@@ -1042,340 +828,13 @@
 }</t>
   </si>
   <si>
-    <t>获取楼宇同步数据列表</t>
-  </si>
-  <si>
-    <t>{
-  Building(cond:"", authInfo:"", order:"")
-  {
-    sourceId
-    name
-    description
-    id
-    _isPartOf
-    type
-  }
-}</t>
-  </si>
-  <si>
-    <t>通过楼宇获取楼层列表</t>
-  </si>
-  <si>
-    <t>根据楼层获取区域同步数据</t>
-  </si>
-  <si>
-    <t>{
-  Building(cond:"{sourceId:{_eq:\"1\"}}", authInfo:"", order:"")
-  {
-    sourceId
-    name
-    description
-    id
-    _isPartOf
-    type
-    hasPart_Floor(cond:"", authInfo:"", order:"")
-    {
-      sourceId
-      name
-      description
-      id
-      _isPartOf
-      type
-    }
-  }
-}</t>
-  </si>
-  <si>
-    <t>{
-  Floor(cond:"{sourceId:{_eq:\"1\"}}", authInfo:"", order:"")
-  {
-    sourceId
-    name
-    description
-    id
-    _isPartOf
-    type
-    hasPart_Room(cond:"", authInfo:"", order:"")
-    {
-      sourceId
-      name
-      description
-      id
-      _isPartOf
-      type
-    }
-  }
-}</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>通过区域code获取设备列表
-Room-&gt;EquipmentLocation-&gt;Equipment-&gt;Point-&gt;Sensor</t>
-  </si>
-  <si>
-    <t>{
-  Room(cond:"", authInfo:"", order:"")
-  {
-    sourceId
-    name
-    description
-    id
-    _isPartOf
-    type
-    isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
-    {
-      equipment
-      location
-      isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
-      {
-        sourceId
-        name
-        description
-        id
-        _isPartOf
-        type
-        hasPoint_Point(cond:"", authInfo:"", order:"")
-        {
-          sourceId
-          sourceSystem
-          name
-          description
-          id
-          _isPointOf
-          type
-          hasSubClass_Sensor(cond:"", authInfo:"", order:"")
-          {
-            sourceId
-            sourceSystem
-            name
-            description
-            id
-            _isPointOf
-            type
-          }
-        }
-      }
-    }
-  }
-}</t>
-  </si>
-  <si>
-    <t>通过楼层获取设备列表
-Floor-&gt;Room-&gt;EquipmentLocation-&gt;Equipment-&gt;Point-&gt;Sensor</t>
-  </si>
-  <si>
-    <t>{
-  Floor(cond:"", authInfo:"", order:"")
-  {
-    sourceId
-    name
-    description
-    id
-    _isPartOf
-    type
-    hasPart_Room(cond:"", authInfo:"", order:"")
-    {
-      sourceId
-      name
-      description
-      id
-      _isPartOf
-      type
-      isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
-      {
-        equipment
-        location
-        isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
-        {
-          sourceId
-          name
-          description
-          id
-          _isPartOf
-          type
-          hasPoint_Point(cond:"", authInfo:"", order:"")
-          {
-            sourceId
-            sourceSystem
-            name
-            description
-            id
-            _isPointOf
-            type
-            hasSubClass_Sensor(cond:"", authInfo:"", order:"")
-            {
-              sourceId
-              sourceSystem
-              name
-              description
-              id
-              _isPointOf
-              type
-            }
-          }
-        }
-      }
-    }
-  }
-}</t>
-  </si>
-  <si>
     <t>获取会议室模式</t>
   </si>
   <si>
-    <t>获取设备实时数据</t>
-  </si>
-  <si>
-    <t>获取实时/时间段内指定占用传感器数据
-Equipment(device_id in [])-&gt;Point-&gt;Sensor-&gt;SensorData(ctime)</t>
-  </si>
-  <si>
     <t>Equipment</t>
   </si>
   <si>
-    <t>获取每小时温度传感器数值</t>
-  </si>
-  <si>
-    <t>{
-  Equipment(cond:"{device_id: {_in: [\"\"]}}", authInfo:"", order:"")
-  {
-    sourceId
-    name
-    description
-    id
-    _isPartOf
-    type
-    hasPoint_Point(cond:"", authInfo:"", order:"")
-    {
-      sourceId
-      sourceSystem
-      name
-      description
-      id
-      _isPointOf
-      type
-      hasSubClass_Sensor(cond:"", authInfo:"", order:"")
-      {
-        sourceId
-        sourceSystem
-        name
-        description
-        id
-        _isPointOf
-        type
-        has_SensorData(cond:"{captureTime:{_gte:\"2022-03-20 03:48:28\", _lte:\"2022-04-20 03:48:28\"}}", authInfo:"", order:"")
-        {
-          ctime
-          sourceSystem
-          id
-          value
-          sensorId
-          type
-        }
-      }
-    }
-  }
-}</t>
-  </si>
-  <si>
-    <t>{
-  Sensor(cond:"{type: {_eq: \"CO2_Sensor\"}}", authInfo:"", order:"")
-  {
-    sourceId
-    sourceSystem
-    name
-    description
-    id
-    _isPointOf
-    type
-    has_SensorData(cond:"{captureTime:{_gte:\"2022-04-20 02:48:29\", _lte:\"2022-04-20 03:48:28\"}}", authInfo:"", order:"")
-    {
-      captureTime
-      sourceSystem
-      id
-      value
-      sensorId
-      type
-    }
-  }
-}</t>
-  </si>
-  <si>
     <t>Sensor</t>
-  </si>
-  <si>
-    <t>获取每小时CO2传感器数值</t>
-  </si>
-  <si>
-    <t>获取每小时PM2.5传感器数值</t>
-  </si>
-  <si>
-    <t>获取每小时TVOC传感器数值</t>
-  </si>
-  <si>
-    <t>获取每小时湿度传感器数值</t>
-  </si>
-  <si>
-    <t>获取设备能耗信息</t>
   </si>
   <si>
     <t>反控风速</t>
@@ -1411,9 +870,6 @@
         reserved_field_2
     }
 }</t>
-  </si>
-  <si>
-    <t>21</t>
   </si>
   <si>
     <t>{
@@ -4877,6 +4333,833 @@
     }
   }
 }</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-21</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-22</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-23</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-24</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-25</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-26</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-27</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-28</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-29</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-30</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-31</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-32</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-33</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-34</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-35</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-36</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-37</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-38</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-39</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-40</t>
+  </si>
+  <si>
+    <t>databrain-queryPostgresqlData-test-41</t>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"", authInfo:"", order:"")
+  {
+    sourceId
+    name
+    description
+    id
+    _isPartOf
+    type
+    hasPart_Room(cond:"", authInfo:"", order:"")
+    {
+      sourceId
+      name
+      description
+      id
+      _isPartOf
+      type
+      isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
+      {
+        sourceId
+        name
+        description
+        equipment
+        _isPartOf
+        location
+        type
+        isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
+        {
+          sourceId
+          name
+          description
+          id
+          _isPartOf
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Building(cond:"", authInfo:"", order:"")
+  {
+    sourceId
+    name
+    description
+    id
+    _isPartOf
+    type
+    hasPart_Floor(cond:"", authInfo:"", order:"")
+    {
+      sourceId
+      name
+      description
+      id
+      _isPartOf
+      type
+      hasPart_Room(cond:"", authInfo:"", order:"")
+      {
+        sourceId
+        name
+        description
+        id
+        _isPartOf
+        type
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Building(cond:"{id:{_eq:\"63737ed7483548ee9cef9c0639ffe515\"}}", authInfo:"", order:"")
+  {
+    sourceId
+    name
+    description
+    id
+    _isPartOf
+    type
+    hasPart_Floor(cond:"", authInfo:"", order:"")
+    {
+      sourceId
+      name
+      description
+      id
+      _isPartOf
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"{id:{_eq:\"b241684da4544ff1b5647dadbd8a9f74\"}}", authInfo:"", order:"")
+  {
+    sourceId
+    name
+    description
+    id
+    _isPartOf
+    type
+    hasPart_Room(cond:"", authInfo:"", order:"")
+    {
+      sourceId
+      name
+      description
+      id
+      _isPartOf
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"{id:{_eq:\"b241684da4544ff1b5647dadbd8a9f74\"}}", authInfo:"", order:"")
+  {
+    sourceId
+    name
+    description
+    id
+    _isPartOf
+    type
+    hasPart_Room(cond:"", authInfo:"", order:"")
+    {
+      sourceId
+      name
+      description
+      id
+      _isPartOf
+      type
+      isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
+      {
+        sourceId
+        name
+        description
+        equipment
+        _isPartOf
+        location
+        type
+        isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
+        {
+          sourceId
+          name
+          description
+          id
+          _isPartOf
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Room(cond:"{id:{_eq:\"c5bc86b0cb2046feaee237fe0f18e8f7\"}}", authInfo:"", order:"")
+  {
+    sourceId
+    name
+    description
+    id
+    _isPartOf
+    type
+    isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
+    {
+      sourceId
+      name
+      description
+      equipment
+      _isPartOf
+      location
+      type
+      isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
+      {
+        sourceId
+        name
+        description
+        id
+        _isPartOf
+        type
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"", authInfo:"", order:"")
+  {
+    sourceId
+    name
+    description
+    id
+    _isPartOf
+    type
+    hasPart_Room(cond:"", authInfo:"", order:"")
+    {
+      sourceId
+      name
+      description
+      id
+      _isPartOf
+      type
+      isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
+      {
+        sourceId
+        name
+        description
+        equipment
+        _isPartOf
+        location
+        type
+        isEquipmentLocationOf_Equipment(cond:"{name:{_like:\"%AS_7130%\"}}", authInfo:"", order:"")
+        {
+          sourceId
+          name
+          description
+          id
+          _isPartOf
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Building(cond:"{id:{_eq:\"63737ed7483548ee9cef9c0639ffe515\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasPart_Floor(cond:"", authInfo:"", order:"")
+    {
+      name
+      description
+      id
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"{id:{_eq:\"b241684da4544ff1b5647dadbd8a9f74\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasPart_Room(cond:"", authInfo:"", order:"")
+    {
+      name
+      description
+      id
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Floor(cond:"{id:{_eq:\"b241684da4544ff1b5647dadbd8a9f74\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasPart_Room(cond:"", authInfo:"", order:"")
+    {
+      name
+      description
+      id
+      type
+      isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
+      {
+        equipment
+        location
+        isEquipmentLocationOf_Equipment(cond:"", authInfo:"", order:"")
+        {
+          name
+          description
+          id
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Equipment(cond:"{id: {_in: [\"e3bd355a01e74cdab5001e074d0ee211\"]}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasPoint_Point(cond:"", authInfo:"", order:"")
+    {
+      name
+      description
+      id
+      type
+      hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"2022-04-26T11:00:00\",_lte:\"2022-04-26T11:10:00\"}}", authInfo:"", order:"")
+      {
+        captureTime
+        pointId
+        value
+        type
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Equipment(cond:"{id: {_in: [\"e3bd355a01e74cdab5001e074d0ee211\"]}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasPoint_Point(cond:"", authInfo:"", order:"")
+    {
+      name
+      description
+      id
+      type
+      hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"2022-04-26T11:40:00\",_lte:\"2022-04-26T11:50:00\"}}", authInfo:"", order:"")
+      {
+        captureTime
+        pointId
+        value
+        type
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取设备实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>获取最近10分钟数据</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Equipment(id in [])-&gt;Point-&gt;Timeseries(captureTime)</t>
+    </r>
+  </si>
+  <si>
+    <t>获取设备时间段内指定占用传感器数据
+Equipment(id in [])-&gt;Point-&gt;Timeseries(captureTime)</t>
+  </si>
+  <si>
+    <t>获取每小时温度传感器数值
+Point(type='Temperature_Sensor')-&gt;Timeseries(captureTime)</t>
+  </si>
+  <si>
+    <t>获取每小时TVOC传感器数值
+Point(type='TVOC_Sensor')-&gt;Timeseries(captureTime)</t>
+  </si>
+  <si>
+    <t>获取每小时湿度传感器数值
+Point(type='Humidity_Sensor')-&gt;Timeseries(captureTime)</t>
+  </si>
+  <si>
+    <t>获取每小时能耗传感器数值
+Point(type='Power_Sensor')-&gt;Timeseries(captureTime)</t>
+  </si>
+  <si>
+    <t>{
+  Equipment(cond:"", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasPoint_Point(cond:"{type: {_eq: \"Power_Sensor\"}}", authInfo:"", order:"")
+    {
+      name
+      description
+      id
+      type
+      hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"2022-04-26T11:00:00\",_lte:\"2022-04-26T11:10:00\"}}", authInfo:"", order:"")
+      {
+        captureTime
+        pointId
+        value
+        type
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>Point</t>
+  </si>
+  <si>
+    <t>获取每小时亮度传感器数值
+Point(type='PM25_Sensor')-&gt;Timeseries(captureTime)</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"Temperature_Sensor\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"2022-04-26T11:00:00\",_lte:\"2022-04-26T12:00:00\"}}", authInfo:"", order:"")
+    {
+      captureTime
+      pointId
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"CO2_Sensor\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"2022-04-26T11:00:00\",_lte:\"2022-04-26T12:00:00\"}}", authInfo:"", order:"")
+    {
+      captureTime
+      pointId
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"Luminance_Sensor\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"2022-04-26T11:00:00\",_lte:\"2022-04-26T12:00:00\"}}", authInfo:"", order:"")
+    {
+      captureTime
+      pointId
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"TVOC_Sensor\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"2022-04-26T11:00:00\",_lte:\"2022-04-26T12:00:00\"}}", authInfo:"", order:"")
+    {
+      captureTime
+      pointId
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"Humidity_Sensor\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"2022-04-26T11:00:00\",_lte:\"2022-04-26T12:00:00\"}}", authInfo:"", order:"")
+    {
+      captureTime
+      pointId
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"Power_Sensor\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"2022-04-26T11:00:00\",_lte:\"2022-04-26T12:00:00\"}}", authInfo:"", order:"")
+    {
+      captureTime
+      pointId
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>通过区域code获取设备列表
+Room(id=)-&gt;EquipmentLocation</t>
+  </si>
+  <si>
+    <t>{
+  Room(cond:"{id:{_eq:\"c5bc86b0cb2046feaee237fe0f18e8f7\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
+    {
+      name
+      description
+      equipment
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>通过楼层获取设备列表
+Floor(id=)-&gt;Room-&gt;EquipmentLocation</t>
+  </si>
+  <si>
+    <t>获取会议室模式
+Room-&gt;EquipmentLocation-&gt;Equipment(id=)-&gt;Point-&gt;Mode_Command-&gt;Mode_Option</t>
+  </si>
+  <si>
+    <t>{
+  Room(cond:"", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    isLocationOf_EquipmentLocation(cond:"", authInfo:"", order:"")
+    {
+      name
+      description
+      equipment
+      type
+      isEquipmentLocationOf_Equipment(cond:"{id:{_eq:\"29b68e62ac3046d39434f06592c42eb8\"}}", authInfo:"", order:"")
+      {
+        name
+        description
+        id
+        type
+        hasPoint_Point(cond:"", authInfo:"", order:"")
+        {
+          name
+          description
+          id
+          type
+          hasSubClass_Mode_Command(cond:"", authInfo:"", order:"")
+          {
+            floorId
+            spaceId
+            name
+            description
+            id
+            type
+            hasAssociatedTag_Mode_Option(cond:"", authInfo:"", order:"")
+            {
+              objectorproperty_id
+              descriptor
+              id
+              value
+            }
+          }
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取每小时CO2传感器数值
+Point(type='CO2_Sensor')-&gt;Timeseries(captureTime)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>建议不用Floor，直接用point id</t>
+    </r>
+  </si>
+  <si>
+    <t>获取设备能耗信息
+Equipment(id)-&gt;Point(type='Power_Sensor')-&gt;Timeseries(captureTime)</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Mode_Command_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_121635069.BlsCmd_Present_Value.Height",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>update 会议室模式
+Mode_Command</t>
+  </si>
+  <si>
+    <t>update 灯
+Luminance_Setpoint</t>
+  </si>
+  <si>
+    <t>update 窗帘开合度
+Position_Command</t>
+  </si>
+  <si>
+    <t>update空调风速
+Speed_Setpoint</t>
+  </si>
+  <si>
+    <t>Update空调温度
+Temperature_Setpoint</t>
+  </si>
+  <si>
+    <t>Update 空调模式
+Mode_Command</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Luminance_Setpoint_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_121635069.BlsCmd_Present_Value.Height",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Position_Command_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_121635069.BlsCmd_Present_Value.Height",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Speed_Setpoint_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_121635069.BlsCmd_Present_Value.Height",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Temperature_Setpoint_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_121635069.BlsCmd_Present_Value.Height",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>rspCodeOfDatasource</t>
+  </si>
+  <si>
+    <t>dataBrainRehearsal_decigoccConnector</t>
+  </si>
+  <si>
+    <t>rspMessageOfDatasource</t>
+  </si>
+  <si>
+    <t>Mode_Command</t>
+  </si>
+  <si>
+    <t>Luminance_Setpoint</t>
+  </si>
+  <si>
+    <t>Position_Command</t>
+  </si>
+  <si>
+    <t>Speed_Setpoint</t>
+  </si>
+  <si>
+    <t>Temperature_Setpoint</t>
   </si>
 </sst>
 </file>
@@ -4965,7 +5248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4991,9 +5274,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5001,18 +5281,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -6045,901 +6313,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95BF81D-F35A-4340-837F-62C66C86E4D8}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.88671875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="57" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="12">
-        <v>200</v>
-      </c>
-      <c r="F2" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E3" s="12">
-        <v>200</v>
-      </c>
-      <c r="F3" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="E4" s="12">
-        <v>200</v>
-      </c>
-      <c r="F4" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="12">
-        <v>200</v>
-      </c>
-      <c r="F5" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="12">
-        <v>200</v>
-      </c>
-      <c r="F6" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="12">
-        <v>200</v>
-      </c>
-      <c r="F7" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" s="12">
-        <v>200</v>
-      </c>
-      <c r="F8" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="12">
-        <v>200</v>
-      </c>
-      <c r="F9" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12">
-        <v>200</v>
-      </c>
-      <c r="F10" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="12">
-        <v>200</v>
-      </c>
-      <c r="F11" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="12">
-        <v>200</v>
-      </c>
-      <c r="F12" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="12">
-        <v>200</v>
-      </c>
-      <c r="F13" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="12">
-        <v>200</v>
-      </c>
-      <c r="F14" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="12">
-        <v>200</v>
-      </c>
-      <c r="F15" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="E16" s="12">
-        <v>200</v>
-      </c>
-      <c r="F16" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E17" s="12">
-        <v>200</v>
-      </c>
-      <c r="F17" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="12">
-        <v>200</v>
-      </c>
-      <c r="F18" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E19" s="12">
-        <v>200</v>
-      </c>
-      <c r="F19" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E20" s="12">
-        <v>200</v>
-      </c>
-      <c r="F20" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="12">
-        <v>200</v>
-      </c>
-      <c r="F21" s="12">
-        <v>100000</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E22" s="16">
-        <v>200</v>
-      </c>
-      <c r="F22" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="E23" s="16">
-        <v>200</v>
-      </c>
-      <c r="F23" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E24" s="16">
-        <v>200</v>
-      </c>
-      <c r="F24" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E25" s="16">
-        <v>200</v>
-      </c>
-      <c r="F25" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="E26" s="16">
-        <v>200</v>
-      </c>
-      <c r="F26" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16">
-        <v>200</v>
-      </c>
-      <c r="F27" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16">
-        <v>200</v>
-      </c>
-      <c r="F28" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="E29" s="16">
-        <v>200</v>
-      </c>
-      <c r="F29" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="E30" s="16">
-        <v>200</v>
-      </c>
-      <c r="F30" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="E31" s="16">
-        <v>200</v>
-      </c>
-      <c r="F31" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16">
-        <v>200</v>
-      </c>
-      <c r="F32" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16">
-        <v>200</v>
-      </c>
-      <c r="F33" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="16">
-        <v>200</v>
-      </c>
-      <c r="F34" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="16">
-        <v>200</v>
-      </c>
-      <c r="F35" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="16">
-        <v>200</v>
-      </c>
-      <c r="F36" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="16">
-        <v>200</v>
-      </c>
-      <c r="F37" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="16">
-        <v>200</v>
-      </c>
-      <c r="F38" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="16">
-        <v>200</v>
-      </c>
-      <c r="F39" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="16">
-        <v>200</v>
-      </c>
-      <c r="F40" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="16">
-        <v>200</v>
-      </c>
-      <c r="F41" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED2918E-9956-4AEF-9D0A-B5DEF5912792}">
-  <dimension ref="A1:H22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="6" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="9" customWidth="1"/>
     <col min="2" max="2" width="33.77734375" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.88671875" style="9" bestFit="1" customWidth="1"/>
@@ -6973,535 +6355,1578 @@
         <v>4</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="12">
+        <v>200</v>
+      </c>
+      <c r="F2" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3" s="12">
+        <v>200</v>
+      </c>
+      <c r="F3" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="E4" s="12">
+        <v>200</v>
+      </c>
+      <c r="F4" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E5" s="12">
+        <v>200</v>
+      </c>
+      <c r="F5" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E6" s="12">
+        <v>200</v>
+      </c>
+      <c r="F6" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7" s="12">
+        <v>200</v>
+      </c>
+      <c r="F7" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="E8" s="12">
+        <v>200</v>
+      </c>
+      <c r="F8" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="12">
+        <v>200</v>
+      </c>
+      <c r="F9" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="12">
+        <v>200</v>
+      </c>
+      <c r="F10" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="12">
+        <v>200</v>
+      </c>
+      <c r="F11" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="12">
+        <v>200</v>
+      </c>
+      <c r="F12" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="12">
+        <v>200</v>
+      </c>
+      <c r="F13" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="12">
+        <v>200</v>
+      </c>
+      <c r="F14" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="12">
+        <v>200</v>
+      </c>
+      <c r="F15" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="12">
+        <v>200</v>
+      </c>
+      <c r="F16" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" s="12">
+        <v>200</v>
+      </c>
+      <c r="F17" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="12">
+        <v>200</v>
+      </c>
+      <c r="F18" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="12">
+        <v>200</v>
+      </c>
+      <c r="F19" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="12">
+        <v>200</v>
+      </c>
+      <c r="F20" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="12">
+        <v>200</v>
+      </c>
+      <c r="F21" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="15">
+        <v>200</v>
+      </c>
+      <c r="F22" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="15">
+        <v>200</v>
+      </c>
+      <c r="F23" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" s="15">
+        <v>200</v>
+      </c>
+      <c r="F24" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="B25" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="15">
+        <v>200</v>
+      </c>
+      <c r="F25" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="15">
+        <v>200</v>
+      </c>
+      <c r="F26" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15">
+        <v>200</v>
+      </c>
+      <c r="F27" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" s="15">
+        <v>200</v>
+      </c>
+      <c r="F28" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" s="15">
+        <v>200</v>
+      </c>
+      <c r="F29" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="15">
+        <v>200</v>
+      </c>
+      <c r="F30" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="E31" s="15">
+        <v>200</v>
+      </c>
+      <c r="F31" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="15">
+        <v>200</v>
+      </c>
+      <c r="F32" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" s="15">
+        <v>200</v>
+      </c>
+      <c r="F33" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E34" s="15">
+        <v>200</v>
+      </c>
+      <c r="F34" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="E35" s="15">
+        <v>200</v>
+      </c>
+      <c r="F35" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E36" s="15">
+        <v>200</v>
+      </c>
+      <c r="F36" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="B37" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" s="15">
+        <v>200</v>
+      </c>
+      <c r="F37" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E38" s="15">
+        <v>200</v>
+      </c>
+      <c r="F38" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="15">
+        <v>200</v>
+      </c>
+      <c r="F39" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E40" s="15">
+        <v>200</v>
+      </c>
+      <c r="F40" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="15">
+        <v>200</v>
+      </c>
+      <c r="F41" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E42" s="15">
+        <v>200</v>
+      </c>
+      <c r="F42" s="15">
+        <v>100000</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED2918E-9956-4AEF-9D0A-B5DEF5912792}">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="93.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="E2" s="20">
-        <v>200</v>
-      </c>
-      <c r="F2" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" s="18" t="s">
+      <c r="D2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="12">
+        <v>200</v>
+      </c>
+      <c r="F2" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="E3" s="20">
-        <v>200</v>
-      </c>
-      <c r="F3" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="C4" s="18" t="s">
+      <c r="D3" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="12">
+        <v>200</v>
+      </c>
+      <c r="F3" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" s="12">
+        <v>200</v>
+      </c>
+      <c r="F4" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="E4" s="20">
-        <v>200</v>
-      </c>
-      <c r="F4" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="E5" s="20">
-        <v>200</v>
-      </c>
-      <c r="F5" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="E6" s="20">
-        <v>200</v>
-      </c>
-      <c r="F6" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20">
-        <v>200</v>
-      </c>
-      <c r="F7" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="20"/>
-    </row>
-    <row r="8" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B8" s="18" t="s">
+      <c r="B5" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="E5" s="12">
+        <v>200</v>
+      </c>
+      <c r="F5" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="12">
+        <v>200</v>
+      </c>
+      <c r="F6" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E7" s="12">
+        <v>200</v>
+      </c>
+      <c r="F7" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E8" s="12">
+        <v>200</v>
+      </c>
+      <c r="F8" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="E9" s="12">
+        <v>200</v>
+      </c>
+      <c r="F9" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="E10" s="12">
+        <v>200</v>
+      </c>
+      <c r="F10" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="E11" s="12">
+        <v>200</v>
+      </c>
+      <c r="F11" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" s="12">
+        <v>200</v>
+      </c>
+      <c r="F12" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="12">
+        <v>200</v>
+      </c>
+      <c r="F13" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="E8" s="20">
-        <v>200</v>
-      </c>
-      <c r="F8" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="E9" s="20">
-        <v>200</v>
-      </c>
-      <c r="F9" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="E10" s="20">
-        <v>200</v>
-      </c>
-      <c r="F10" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="E11" s="20">
-        <v>200</v>
-      </c>
-      <c r="F11" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B12" s="18" t="s">
+      <c r="E14" s="12">
+        <v>200</v>
+      </c>
+      <c r="F14" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="E12" s="20">
-        <v>200</v>
-      </c>
-      <c r="F12" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="B13" s="18" t="s">
+      <c r="C15" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="E15" s="12">
+        <v>200</v>
+      </c>
+      <c r="F15" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="E13" s="20">
-        <v>200</v>
-      </c>
-      <c r="F13" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="E14" s="20">
-        <v>200</v>
-      </c>
-      <c r="F14" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="E15" s="20">
-        <v>200</v>
-      </c>
-      <c r="F15" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="E16" s="20">
-        <v>200</v>
-      </c>
-      <c r="F16" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="E17" s="20">
-        <v>200</v>
-      </c>
-      <c r="F17" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="E18" s="20">
-        <v>200</v>
-      </c>
-      <c r="F18" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="E19" s="20">
-        <v>200</v>
-      </c>
-      <c r="F19" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="19" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B20" s="18" t="s">
+      <c r="E16" s="12">
+        <v>200</v>
+      </c>
+      <c r="F16" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="E17" s="12">
+        <v>200</v>
+      </c>
+      <c r="F17" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="E18" s="12">
+        <v>200</v>
+      </c>
+      <c r="F18" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="E19" s="12">
+        <v>200</v>
+      </c>
+      <c r="F19" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="E20" s="12">
+        <v>200</v>
+      </c>
+      <c r="F20" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="E21" s="12">
+        <v>200</v>
+      </c>
+      <c r="F21" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="E20" s="20">
-        <v>200</v>
-      </c>
-      <c r="F20" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="E21" s="20">
-        <v>200</v>
-      </c>
-      <c r="F21" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="E22" s="20">
-        <v>200</v>
-      </c>
-      <c r="F22" s="20">
-        <v>100000</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>225</v>
+      <c r="B22" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="E22" s="12">
+        <v>200</v>
+      </c>
+      <c r="F22" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test cases for smart space realtime function
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C37F3F0-9E9B-42E8-8E18-CC4CB70B65C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE2F8E7-D0BA-4CB2-BC12-AA34BCA8C7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
     <sheet name="getDataGraphQL" sheetId="3" r:id="rId2"/>
     <sheet name="queryPostgresqlData-backup" sheetId="4" r:id="rId3"/>
-    <sheet name="verifySmartSpaceFunction" sheetId="5" r:id="rId4"/>
+    <sheet name="verifySmartSpaceFunction-bc" sheetId="5" r:id="rId4"/>
+    <sheet name="verifySmartSpaceOtherFunc" sheetId="6" r:id="rId5"/>
+    <sheet name="verifySmartSpaceRealtimeFunc" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">verifySmartSpaceFunction!$A$1:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'verifySmartSpaceFunction-bc'!$A$1:$G$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="442">
   <si>
     <t>description</t>
   </si>
@@ -5599,12 +5601,1535 @@
     }
 }</t>
   </si>
+  <si>
+    <t>{
+  Equipment(cond:"{id:{_in:[\"e3bd355a01e74cdab5001e074d0ee211\",\"29b68e62ac3046d39434f06592c42eb8\",\"a65aa46d3fdd48abb586092a9a650dd2\",\"b896501c1e874f8487871b4c67597c1d\",\"5242339816e84bf381a698c709430650\",\"ad776315e61d42a58c30e6f9ebd19d52\"]}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasPoint_Point(cond:"{type:{_eq:\"CO2_Sensor\"}}", authInfo:"", order:"")
+    {
+      name
+      description
+      id
+      type
+      hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"2022-05-18T19:00:00\", _lte:\"2022-05-18T19:30:00\"}}", authInfo:"", order:"captureTime DESC")
+      {
+        captureTime
+        id
+        value
+        type
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>Equipment-&gt; hasPoint_Point-&gt; hasTimeseries_Timeseries</t>
+  </si>
+  <si>
+    <t>根据日期获取CO2传感器数值并按“captureTime 降序”排序
+Equipment(id in [])-&gt;Point(type=)-&gt;Timeseries(captureTime)</t>
+  </si>
+  <si>
+    <t>databrain-smartspace-test-32</t>
+  </si>
+  <si>
+    <t>databrain-smartspace-test-33</t>
+  </si>
+  <si>
+    <t>根据日期获取CO2传感器数值并按“captureTime 升序”排序
+Equipment(id in [])-&gt;Point(type=)-&gt;Timeseries(captureTime)</t>
+  </si>
+  <si>
+    <t>{
+  Equipment(cond:"{id:{_in:[\"e3bd355a01e74cdab5001e074d0ee211\",\"29b68e62ac3046d39434f06592c42eb8\",\"a65aa46d3fdd48abb586092a9a650dd2\",\"b896501c1e874f8487871b4c67597c1d\",\"5242339816e84bf381a698c709430650\",\"ad776315e61d42a58c30e6f9ebd19d52\"]}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasPoint_Point(cond:"{type:{_eq:\"CO2_Sensor\"}}", authInfo:"", order:"")
+    {
+      name
+      description
+      id
+      type
+      hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"2022-05-18T19:00:00\", _lte:\"2022-05-18T19:30:00\"}}", authInfo:"", order:"captureTime ASC")
+      {
+        captureTime
+        id
+        value
+        type
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>Point-&gt;hasTimeseries_TimeseriesConnection-&gt;edges</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Mode_Command（空调模式）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Mode_Command',id='')-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
+  </si>
+  <si>
+    <t>sqlStatement</t>
+  </si>
+  <si>
+    <t>System1:GmsDevice_4_7130_1082130448.Present_Value.Height</t>
+  </si>
+  <si>
+    <t>System1:GmsDevice_4_7130_121634835.RAQual_Present_Value</t>
+  </si>
+  <si>
+    <t>System1:GmsDevice_4_7130_16777322.Present_Value</t>
+  </si>
+  <si>
+    <t>System1:GmsDevice_4_7130_121634835.RHuRel_Present_Value</t>
+  </si>
+  <si>
+    <t>System1:GmsDevice_4_7130_1090519068.Present_Value</t>
+  </si>
+  <si>
+    <t>System1:GmsDevice_4_7130_121634870.PltOpMod_Relinquish_Default</t>
+  </si>
+  <si>
+    <t>System1:GmsDevice_1_7105_29360128.Present_Value</t>
+  </si>
+  <si>
+    <t>System1:GmsDevice_4_7130_79692330.Present_Value</t>
+  </si>
+  <si>
+    <t>System1:GmsDevice_4_7130_121634914.FanMultiSpd_Present_Value</t>
+  </si>
+  <si>
+    <t>System1:GmsDevice_4_7130_121634835.RTemp_Present_Value</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"CO2_Sensor\"}},{id: {_eq: \"5d11b970dfdb4b4fb68c20af04fa87af\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634835.RAQual_Present_Value' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取CO2_Sensor（室内co2(ppm))实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='CO2_Sensor',id='')-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Mode_Command\"}},{id: {_eq: \"67ac53b928a947fc9afcb29f30cce93f\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Mode_Command\"}},{id: {_eq: \"22a30930ce1d4007a59e24bef925d17d\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Mode_Command\"}},{id: {_eq: \"858e767d499343bb9198ff4603db79fb\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"GreenLeaf_Mode_Command\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime DESC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_16777322.Present_Value' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Humidity_Sensor（室内湿度%rh）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">按时间升序（captureTime ASC）排序
+添加了分页功能：
+pageIndex:1
+pageSize:10
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Humidity_Sensorr',id='')-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Humidity_Sensor\"}},{id: {_eq: \"9e4ab0cc4fb24f40ad8b80facdeb017b\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_TimeseriesConnection(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC", after:"1", first:10)
+    {
+      totalElements
+      totalPages
+      pageSize
+      page
+      numberOfElements
+      edges {
+        node {
+          captureTime
+          id
+          value
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634835.RHuRel_Present_Value' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC LIMIT 10</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Mode_Command（会议模式）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">按时间升序（captureTime ASC）排序
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Mode_Command',id='')-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Mode_Command（会议模式）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Mode_Command',id='')-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Position_Command（窗帘控制）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Position_Command')-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Speed_Setpoint（风机速度）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Speed_Setpoint)-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Temperature_Sensor（"室内温度℃）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Temperature_Sensor',id='')-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Temperature_Setpoint（温度设定℃）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Temperature_Setpoint')-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"Position_Command\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"Speed_Setpoint\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Temperature_Sensor\"}},{id: {_eq: \"ec2510822ef64bebac25f028bd3e147c\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"Temperature_Setpoint\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634870.PltOpMod_Relinquish_Default' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_1_7105_29360128.Present_Value' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_79692330.Present_Value' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_1082130448.Present_Value.Height' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634914.FanMultiSpd_Present_Value' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634835.RTemp_Present_Value' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Luminance_Setpoint（灯光控制）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">按时间升序（captureTime DESC）排序
+添加了分页功能：
+pageIndex:1
+pageSize:10
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Luminance_Setpoint')-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"Luminance_Setpoint\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_TimeseriesConnection(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime DESC", after:"1", first:10)
+    {
+      totalElements
+      totalPages
+      pageSize
+      page
+      numberOfElements
+      edges {
+        node {
+          captureTime
+          id
+          value
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_1090519068.Present_Value' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC  LIMIT 10</t>
+  </si>
+  <si>
+    <t>System1:GmsDevice_4_7130_121634849.SpTR_Present_Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634849.SpTR_Present_Value' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Luminance_Sensor\"}},{id: {_eq: \"e5f0eb45ff8f47dd800214e56a2b6eef\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Occupancy_Status\"}},{id: {_eq: \"6bcccd43f94246098510735605bd0cf7\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime DESC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"Power_Sensor\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_TimeseriesConnection(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC", after:"1", first:10)
+    {
+      totalElements
+      totalPages
+      pageSize
+      page
+      numberOfElements
+      edges {
+        node {
+          captureTime
+          id
+          value
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Temperature_Sensor\"}},{id: {_eq: \"b20b01a19aa8455f8d9275d32a1450dd\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_TimeseriesConnection(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime DESC", after:"1", first:10)
+    {
+      totalElements
+      totalPages
+      pageSize
+      page
+      numberOfElements
+      edges {
+        node {
+          captureTime
+          id
+          value
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Luminance_Sensor（Sensor48c775 Luminance)实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Luminance_Sensor',id='')-&gt;Timeseries(captureTime)
+sourcesystem:Enlighted</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Occupancy_Status（ROOM ssi Occupancy Status）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间降序（captureTime DESC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Occupancy_Status',id='')-&gt;Timeseries(captureTime)
+sourcesystem:Enlighted</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Power_Sensor（Sensor48c775 Power）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">按时间升序（captureTime ASC）排序
+添加了分页功能：
+pageIndex:1
+pageSize:10
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Power_Sensor')-&gt;Timeseries(captureTime)
+sourcesystem:Enlighted</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Temperature_Sensor（Sensor48c775 Temperature）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">按时间升序（captureTime DESC）排序
+添加了分页功能：
+pageIndex:1
+pageSize:10
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Temperature_Sensor',id='')-&gt;Timeseries(captureTime)
+sourcesystem:Enlighted</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,lightLevel as Value,id as PropertyId,sourceSystem from EnlightedValue ev where id = '2' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t>sid</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>5d11b970dfdb4b4fb68c20af04fa87af</t>
+  </si>
+  <si>
+    <t>095a804d31584d4bb7762ade3d1b3047</t>
+  </si>
+  <si>
+    <t>9e4ab0cc4fb24f40ad8b80facdeb017b</t>
+  </si>
+  <si>
+    <t>73b97708f1404419a1e10b31baba725a</t>
+  </si>
+  <si>
+    <t>67ac53b928a947fc9afcb29f30cce93f</t>
+  </si>
+  <si>
+    <t>22a30930ce1d4007a59e24bef925d17d</t>
+  </si>
+  <si>
+    <t>858e767d499343bb9198ff4603db79fb</t>
+  </si>
+  <si>
+    <t>0db848bd91874e8aac289a03b5e18c6b</t>
+  </si>
+  <si>
+    <t>e248aeb1cdb74be2b3f0b9957ea3d6f5</t>
+  </si>
+  <si>
+    <t>ec2510822ef64bebac25f028bd3e147c</t>
+  </si>
+  <si>
+    <t>c873ae9f77a54bf2af2b91d924038cfd</t>
+  </si>
+  <si>
+    <t>e5f0eb45ff8f47dd800214e56a2b6eef</t>
+  </si>
+  <si>
+    <t>6bcccd43f94246098510735605bd0cf7</t>
+  </si>
+  <si>
+    <t>c39df126e6b54469adf4b4a00b703ef4</t>
+  </si>
+  <si>
+    <t>b20b01a19aa8455f8d9275d32a1450dd</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,temperature as Value,id as PropertyId,sourceSystem from EnlightedValue ev where id = '2' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC  LIMIT 10</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,value as Value,id as PropertyId,sourceSystem from EnlightedOccupancyStatus eos where id = '1' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"CO2_Sensor\"}},{id: {_eq: \"abd4823004544adab6b2a8ed92ca6b33\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>abd4823004544adab6b2a8ed92ca6b33</t>
+  </si>
+  <si>
+    <t>24e124128a486491</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,power as Value,id as PropertyId,sourceSystem from EnlightedValue ev where id = '2' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC LIMIT 10</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取CO2_Sensor（Building F Floor 1 CO2 Sensor 1)实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='CO2_Sensor',id='')-&gt;Timeseries(captureTime)
+sourcesystem:iotgateway</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,co2 as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取GreenLeaf_Mode_Command（绿叶模式）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间降序（captureTime DESC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='GreenLeaf_Mode_Command')-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Humidity_Sensor\"}},{id: {_eq: \"63fc159fb0b3419ca1bd14d86eaf43e9\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime DESC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>63fc159fb0b3419ca1bd14d86eaf43e9</t>
+  </si>
+  <si>
+    <t>394edf421c4a43da941b9002bc942f60</t>
+  </si>
+  <si>
+    <t>ad776315e61d42a58c30e6f9ebd19d52</t>
+  </si>
+  <si>
+    <t>24e124600b251195</t>
+  </si>
+  <si>
+    <t>9bcccd24f94246098510735605bd9db6</t>
+  </si>
+  <si>
+    <t>24e124538b441301</t>
+  </si>
+  <si>
+    <t>2d182a01a6bb4bef920fc08debac2f69</t>
+  </si>
+  <si>
+    <t>5540e6f7753941908379ddc8ecb43ffd</t>
+  </si>
+  <si>
+    <t>87cebf00987844849ad130af5fe39971</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Luminance_Sensor\"}},{id: {_eq: \"394edf421c4a43da941b9002bc942f60\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_TimeseriesConnection(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC", after:"1", first:10)
+    {
+      totalElements
+      totalPages
+      pageSize
+      page
+      numberOfElements
+      edges {
+        node {
+          captureTime
+          id
+          value
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Occupancy_Sensor（灯光控制）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">按时间升序（captureTime DESC）排序
+添加了分页功能：
+pageIndex:1
+pageSize:10
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Occupancy_Sensor')-&gt;Timeseries(captureTime)
+sourcesystem:iotgateway</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"Occupancy_Sensor\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_TimeseriesConnection(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime DESC", after:"1", first:10)
+    {
+      totalElements
+      totalPages
+      pageSize
+      page
+      numberOfElements
+      edges {
+        node {
+          captureTime
+          id
+          value
+          type
+        }
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,humidity as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Humidity_Sensor（Building F Floor 1 Humidity Sensor 1）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">按时间降序（captureTime DESC）排序
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Humidity_Sensor',id='')-&gt;Timeseries(captureTime)
+sourcesystem:iotgateway</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Luminance_Sensor（Building F Floor 1 Pressure Sensor 1）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">按时间升序（captureTime ASC）排序
+添加了分页功能：
+pageIndex:1
+pageSize:10
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Luminance_Sensor',id='')-&gt;Timeseries(captureTime)
+sourcesystem:iotgateway</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,infrared as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC limit 10</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"Pressure_Sensor\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Temperature_Sensor\"}},{id: {_eq: \"5540e6f7753941908379ddc8ecb43ffd\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{type: {_eq: \"TVOC_Sensor\"}}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,pressure as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Pressure_Sensor（Building F Floor 1 Pressure Sensor 1)实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Pressure_Sensor')-&gt;Timeseries(captureTime)
+sourcesystem:iotgateway</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Temperature_Sensor（Building F Floor 1 Temperature Sensor 1)实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Temperature_Sensor',id='')-&gt;Timeseries(captureTime)
+sourcesystem:iotgateway</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,temperature as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取TVOC_Sensor（Building F Floor 1 Pressure Sensor 1)实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='TVOC_Sensor')-&gt;Timeseries(captureTime)
+sourcesystem:iotgateway</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,tvoc as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,people_counter_all as Value,devEUI as PropertyId,sourceSystem from VS121_Data ad where devEUI = '24e124600b251195' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC limit 10</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Occupancy_Status（)实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Occupancy_Status',id='')-&gt;Timeseries(captureTime)
+sourcesystem:iotgateway</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+  Point(cond:"{_and:[{type: {_eq: \"Occupancy_Status\"}},{id: {_eq: \"9bcccd24f94246098510735605bd9db6\"}}]}", authInfo:"", order:"")
+  {
+    name
+    description
+    id
+    type
+    hasTimeseries_Timeseries(cond:"{captureTime:{_gte:\"$startTime\",_lte:\"$endTime\"}}", authInfo:"", order:"captureTime ASC")
+    {
+      captureTime
+      id
+      value
+      type
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,pir as Value,devEUI as PropertyId,sourceSystem from WS202_Data ad where devEUI = '24e124538b441301' 
+and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Mode_Command_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_1_7105_29360128.Present_Value",
+          value: "0"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Mode_Command_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_79692330.Present_Value",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Position_Command_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_1082130448.Present_Value.Height",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Speed_Setpoint_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_121634914.FanMultiSpd_Present_Value",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Temperature_Setpoint_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_121634849.SpTR_Present_Value",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>"ErrorCode":0</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Mode_Command_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_121634870.PltOpMod_Relinquish_Default",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Luminance_Setpoint_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_1090519068.Present_Value",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>update灯
+Luminance_Setpoint</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5634,6 +7159,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5686,7 +7218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5720,6 +7252,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6753,7 +8288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95BF81D-F35A-4340-837F-62C66C86E4D8}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -7769,10 +9304,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED2918E-9956-4AEF-9D0A-B5DEF5912792}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -8617,6 +10152,1564 @@
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
     </row>
+    <row r="33" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="E33" s="12">
+        <v>200</v>
+      </c>
+      <c r="F33" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+    </row>
+    <row r="34" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="E34" s="12">
+        <v>200</v>
+      </c>
+      <c r="F34" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA4C4C8-01FF-4E34-B41E-A7427C7932E0}">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="66.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="12">
+        <v>200</v>
+      </c>
+      <c r="F2" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="12">
+        <v>200</v>
+      </c>
+      <c r="F3" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" s="12">
+        <v>200</v>
+      </c>
+      <c r="F4" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="E5" s="12">
+        <v>200</v>
+      </c>
+      <c r="F5" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E6" s="12">
+        <v>200</v>
+      </c>
+      <c r="F6" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E7" s="12">
+        <v>200</v>
+      </c>
+      <c r="F7" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E8" s="12">
+        <v>200</v>
+      </c>
+      <c r="F8" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="E9" s="12">
+        <v>200</v>
+      </c>
+      <c r="F9" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="E10" s="12">
+        <v>200</v>
+      </c>
+      <c r="F10" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="E11" s="12">
+        <v>200</v>
+      </c>
+      <c r="F11" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="E12" s="12">
+        <v>200</v>
+      </c>
+      <c r="F12" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E13" s="12">
+        <v>200</v>
+      </c>
+      <c r="F13" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="E14" s="12">
+        <v>200</v>
+      </c>
+      <c r="F14" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="E15" s="12">
+        <v>200</v>
+      </c>
+      <c r="F15" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="E16" s="12">
+        <v>200</v>
+      </c>
+      <c r="F16" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="E17" s="12">
+        <v>200</v>
+      </c>
+      <c r="F17" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="E18" s="12">
+        <v>200</v>
+      </c>
+      <c r="F18" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="E19" s="12">
+        <v>200</v>
+      </c>
+      <c r="F19" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="E20" s="12">
+        <v>200</v>
+      </c>
+      <c r="F20" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="E21" s="12">
+        <v>200</v>
+      </c>
+      <c r="F21" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="E22" s="12">
+        <v>200</v>
+      </c>
+      <c r="F22" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="E23" s="12">
+        <v>200</v>
+      </c>
+      <c r="F23" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="E24" s="12">
+        <v>200</v>
+      </c>
+      <c r="F24" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="10">
+        <v>0</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="E25" s="12">
+        <v>200</v>
+      </c>
+      <c r="F25" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="10">
+        <v>0</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="E26" s="12">
+        <v>200</v>
+      </c>
+      <c r="F26" s="12">
+        <v>100000</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2181B9E2-AEE2-4C11-98DD-ED06134DE024}">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="9" customWidth="1"/>
+    <col min="4" max="4" width="57.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="22" style="9" customWidth="1"/>
+    <col min="7" max="7" width="33.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2" s="12">
+        <v>200</v>
+      </c>
+      <c r="I2" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="H3" s="12">
+        <v>200</v>
+      </c>
+      <c r="I3" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="H4" s="12">
+        <v>200</v>
+      </c>
+      <c r="I4" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="H5" s="12">
+        <v>200</v>
+      </c>
+      <c r="I5" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="H6" s="12">
+        <v>200</v>
+      </c>
+      <c r="I6" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="H7" s="12">
+        <v>200</v>
+      </c>
+      <c r="I7" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="H8" s="12">
+        <v>200</v>
+      </c>
+      <c r="I8" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H9" s="12">
+        <v>200</v>
+      </c>
+      <c r="I9" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="H10" s="12">
+        <v>200</v>
+      </c>
+      <c r="I10" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="H11" s="12">
+        <v>200</v>
+      </c>
+      <c r="I11" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H12" s="12">
+        <v>200</v>
+      </c>
+      <c r="I12" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="F13" s="10">
+        <v>2</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="H13" s="12">
+        <v>200</v>
+      </c>
+      <c r="I13" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="H14" s="12">
+        <v>200</v>
+      </c>
+      <c r="I14" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="F15" s="10">
+        <v>2</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="H15" s="12">
+        <v>200</v>
+      </c>
+      <c r="I15" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="F16" s="10">
+        <v>2</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="H16" s="12">
+        <v>200</v>
+      </c>
+      <c r="I16" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="H17" s="12">
+        <v>200</v>
+      </c>
+      <c r="I17" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="H18" s="12">
+        <v>200</v>
+      </c>
+      <c r="I18" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="H19" s="12">
+        <v>200</v>
+      </c>
+      <c r="I19" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="H20" s="12">
+        <v>200</v>
+      </c>
+      <c r="I20" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="H21" s="12">
+        <v>200</v>
+      </c>
+      <c r="I21" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="H22" s="12">
+        <v>200</v>
+      </c>
+      <c r="I22" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H23" s="12">
+        <v>200</v>
+      </c>
+      <c r="I23" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="H24" s="12">
+        <v>200</v>
+      </c>
+      <c r="I24" s="12">
+        <v>100000</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solve the problem of LocalDateTime
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE2F8E7-D0BA-4CB2-BC12-AA34BCA8C7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABCFCE5-E6FA-4B27-B271-19A546632E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -5750,10 +5750,6 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634835.RAQual_Present_Value' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">获取CO2_Sensor（室内co2(ppm))实时数据
 </t>
@@ -5851,10 +5847,6 @@
     }
   }
 }</t>
-  </si>
-  <si>
-    <t>SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_16777322.Present_Value' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC</t>
   </si>
   <si>
     <r>
@@ -5915,10 +5907,6 @@
 }</t>
   </si>
   <si>
-    <t>SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634835.RHuRel_Present_Value' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC LIMIT 10</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">获取Mode_Command（会议模式）实时数据
 </t>
@@ -6152,30 +6140,6 @@
     }
   }
 }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634870.PltOpMod_Relinquish_Default' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_1_7105_29360128.Present_Value' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_79692330.Present_Value' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_1082130448.Present_Value.Height' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634914.FanMultiSpd_Present_Value' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634835.RTemp_Present_Value' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
   </si>
   <si>
     <r>
@@ -6236,15 +6200,7 @@
 }</t>
   </si>
   <si>
-    <t>SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_1090519068.Present_Value' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC  LIMIT 10</t>
-  </si>
-  <si>
     <t>System1:GmsDevice_4_7130_121634849.SpTR_Present_Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634849.SpTR_Present_Value' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
   </si>
   <si>
     <t>{
@@ -6453,10 +6409,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">SELECT dataLayerTime,lightLevel as Value,id as PropertyId,sourceSystem from EnlightedValue ev where id = '2' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC </t>
-  </si>
-  <si>
     <t>sid</t>
   </si>
   <si>
@@ -6506,14 +6458,6 @@
   </si>
   <si>
     <t>b20b01a19aa8455f8d9275d32a1450dd</t>
-  </si>
-  <si>
-    <t>SELECT dataLayerTime,temperature as Value,id as PropertyId,sourceSystem from EnlightedValue ev where id = '2' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC  LIMIT 10</t>
-  </si>
-  <si>
-    <t>SELECT dataLayerTime,value as Value,id as PropertyId,sourceSystem from EnlightedOccupancyStatus eos where id = '1' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC</t>
   </si>
   <si>
     <t>{
@@ -6538,10 +6482,6 @@
   </si>
   <si>
     <t>24e124128a486491</t>
-  </si>
-  <si>
-    <t>SELECT dataLayerTime,power as Value,id as PropertyId,sourceSystem from EnlightedValue ev where id = '2' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC LIMIT 10</t>
   </si>
   <si>
     <r>
@@ -6569,10 +6509,6 @@
 Point(type='CO2_Sensor',id='')-&gt;Timeseries(captureTime)
 sourcesystem:iotgateway</t>
     </r>
-  </si>
-  <si>
-    <t>SELECT dataLayerTime,co2 as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC</t>
   </si>
   <si>
     <r>
@@ -6732,10 +6668,6 @@
 }</t>
   </si>
   <si>
-    <t>SELECT dataLayerTime,humidity as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">获取Humidity_Sensor（Building F Floor 1 Humidity Sensor 1）实时数据
 </t>
@@ -6795,10 +6727,6 @@
     </r>
   </si>
   <si>
-    <t>SELECT dataLayerTime,infrared as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC limit 10</t>
-  </si>
-  <si>
     <t>{
   Point(cond:"{type: {_eq: \"Pressure_Sensor\"}}", authInfo:"", order:"")
   {
@@ -6851,10 +6779,6 @@
     }
   }
 }</t>
-  </si>
-  <si>
-    <t>SELECT dataLayerTime,pressure as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC</t>
   </si>
   <si>
     <r>
@@ -6911,10 +6835,6 @@
     </r>
   </si>
   <si>
-    <t>SELECT dataLayerTime,temperature as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">获取TVOC_Sensor（Building F Floor 1 Pressure Sensor 1)实时数据
 </t>
@@ -6942,14 +6862,6 @@
     </r>
   </si>
   <si>
-    <t>SELECT dataLayerTime,tvoc as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC</t>
-  </si>
-  <si>
-    <t>SELECT dataLayerTime,people_counter_all as Value,devEUI as PropertyId,sourceSystem from VS121_Data ad where devEUI = '24e124600b251195' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime DESC limit 10</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">获取Occupancy_Status（)实时数据
 </t>
@@ -6995,10 +6907,6 @@
 }</t>
   </si>
   <si>
-    <t>SELECT dataLayerTime,pir as Value,devEUI as PropertyId,sourceSystem from WS202_Data ad where devEUI = '24e124538b441301' 
-and dataLayerTime &gt;= '$startTime' AND dataLayerTime &lt;= '$endTime' order by dataLayerTime ASC</t>
-  </si>
-  <si>
     <t>mutation mutationName{
    Mode_Command_Update(input:
    [
@@ -7123,6 +7031,98 @@
   <si>
     <t>update灯
 Luminance_Setpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634835.RAQual_Present_Value' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_16777322.Present_Value' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime DESC</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634835.RHuRel_Present_Value' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC LIMIT 10</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_1090519068.Present_Value' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime DESC  LIMIT 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634870.PltOpMod_Relinquish_Default' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_1_7105_29360128.Present_Value' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_79692330.Present_Value' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_1082130448.Present_Value.Height' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634914.FanMultiSpd_Present_Value' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634835.RTemp_Present_Value' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,Value,PropertyId,sourceSystem from DesigoccValue dv where PropertyId = 'System1:GmsDevice_4_7130_121634849.SpTR_Present_Value' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT dataLayerTime,lightLevel as Value,id as PropertyId,sourceSystem from EnlightedValue ev where id = '2' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC </t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,value as Value,id as PropertyId,sourceSystem from EnlightedOccupancyStatus eos where id = '1' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime DESC</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,power as Value,id as PropertyId,sourceSystem from EnlightedValue ev where id = '2' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC LIMIT 10</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,temperature as Value,id as PropertyId,sourceSystem from EnlightedValue ev where id = '2' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime DESC  LIMIT 10</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,co2 as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,humidity as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime DESC</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,infrared as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC limit 10</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,people_counter_all as Value,devEUI as PropertyId,sourceSystem from VS121_Data ad where devEUI = '24e124600b251195' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime DESC limit 10</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,pir as Value,devEUI as PropertyId,sourceSystem from WS202_Data ad where devEUI = '24e124538b441301' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,pressure as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,temperature as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC</t>
+  </si>
+  <si>
+    <t>SELECT dataLayerTime,tvoc as Value,devEUI as PropertyId,sourceSystem from AM100_Data ad where devEUI = '24e124128a486491' 
+and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC</t>
   </si>
 </sst>
 </file>
@@ -10213,7 +10213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA4C4C8-01FF-4E34-B41E-A7427C7932E0}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -10715,13 +10715,13 @@
         <v>256</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>441</v>
+        <v>418</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>234</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
       <c r="E20" s="12">
         <v>200</v>
@@ -10736,7 +10736,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10750,7 +10750,7 @@
         <v>233</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="E21" s="12">
         <v>200</v>
@@ -10765,7 +10765,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10779,7 +10779,7 @@
         <v>233</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="E22" s="12">
         <v>200</v>
@@ -10794,7 +10794,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10808,7 +10808,7 @@
         <v>233</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="E23" s="12">
         <v>200</v>
@@ -10823,7 +10823,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10837,7 +10837,7 @@
         <v>235</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
       <c r="E24" s="12">
         <v>200</v>
@@ -10852,7 +10852,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10866,7 +10866,7 @@
         <v>236</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
       <c r="E25" s="12">
         <v>200</v>
@@ -10881,7 +10881,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10895,7 +10895,7 @@
         <v>237</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="E26" s="12">
         <v>200</v>
@@ -10910,7 +10910,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -10924,8 +10924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2181B9E2-AEE2-4C11-98DD-ED06134DE024}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -10956,10 +10956,10 @@
         <v>25</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>325</v>
@@ -10979,7 +10979,7 @@
         <v>238</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>267</v>
@@ -10988,13 +10988,13 @@
         <v>336</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>327</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>337</v>
+        <v>419</v>
       </c>
       <c r="H2" s="12">
         <v>200</v>
@@ -11011,22 +11011,22 @@
         <v>239</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>328</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>343</v>
+        <v>420</v>
       </c>
       <c r="H3" s="12">
         <v>200</v>
@@ -11043,22 +11043,22 @@
         <v>240</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>323</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>329</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>346</v>
+        <v>421</v>
       </c>
       <c r="H4" s="12">
         <v>200</v>
@@ -11075,22 +11075,22 @@
         <v>241</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>323</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>330</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>365</v>
+        <v>422</v>
       </c>
       <c r="H5" s="12">
         <v>200</v>
@@ -11107,22 +11107,22 @@
         <v>242</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>331</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>357</v>
+        <v>423</v>
       </c>
       <c r="H6" s="12">
         <v>200</v>
@@ -11139,22 +11139,22 @@
         <v>243</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>332</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>358</v>
+        <v>424</v>
       </c>
       <c r="H7" s="12">
         <v>200</v>
@@ -11177,16 +11177,16 @@
         <v>267</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>333</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>359</v>
+        <v>425</v>
       </c>
       <c r="H8" s="12">
         <v>200</v>
@@ -11203,22 +11203,22 @@
         <v>245</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>326</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>360</v>
+        <v>426</v>
       </c>
       <c r="H9" s="12">
         <v>200</v>
@@ -11235,22 +11235,22 @@
         <v>246</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>334</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>361</v>
+        <v>427</v>
       </c>
       <c r="H10" s="12">
         <v>200</v>
@@ -11267,22 +11267,22 @@
         <v>247</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>335</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>362</v>
+        <v>428</v>
       </c>
       <c r="H11" s="12">
         <v>200</v>
@@ -11299,22 +11299,22 @@
         <v>248</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>366</v>
-      </c>
       <c r="G12" s="10" t="s">
-        <v>367</v>
+        <v>429</v>
       </c>
       <c r="H12" s="12">
         <v>200</v>
@@ -11331,22 +11331,22 @@
         <v>249</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="F13" s="10">
         <v>2</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>376</v>
+        <v>430</v>
       </c>
       <c r="H13" s="12">
         <v>200</v>
@@ -11363,22 +11363,22 @@
         <v>250</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>395</v>
+        <v>431</v>
       </c>
       <c r="H14" s="12">
         <v>200</v>
@@ -11395,22 +11395,22 @@
         <v>251</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>323</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="F15" s="10">
         <v>2</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>399</v>
+        <v>432</v>
       </c>
       <c r="H15" s="12">
         <v>200</v>
@@ -11427,22 +11427,22 @@
         <v>252</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>323</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="F16" s="10">
         <v>2</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>394</v>
+        <v>433</v>
       </c>
       <c r="H16" s="12">
         <v>200</v>
@@ -11459,22 +11459,22 @@
         <v>253</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>401</v>
+        <v>434</v>
       </c>
       <c r="H17" s="12">
         <v>200</v>
@@ -11491,22 +11491,22 @@
         <v>254</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>416</v>
+        <v>435</v>
       </c>
       <c r="H18" s="12">
         <v>200</v>
@@ -11523,22 +11523,22 @@
         <v>255</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>323</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>419</v>
+        <v>436</v>
       </c>
       <c r="H19" s="12">
         <v>200</v>
@@ -11555,22 +11555,22 @@
         <v>256</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>323</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="H20" s="12">
         <v>200</v>
@@ -11587,22 +11587,22 @@
         <v>257</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>430</v>
+        <v>408</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>431</v>
+        <v>409</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="H21" s="12">
         <v>200</v>
@@ -11619,22 +11619,22 @@
         <v>258</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>423</v>
+        <v>439</v>
       </c>
       <c r="H22" s="12">
         <v>200</v>
@@ -11651,22 +11651,22 @@
         <v>277</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>425</v>
+        <v>406</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>426</v>
+        <v>440</v>
       </c>
       <c r="H23" s="12">
         <v>200</v>
@@ -11683,22 +11683,22 @@
         <v>281</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>427</v>
+        <v>407</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>267</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>428</v>
+        <v>441</v>
       </c>
       <c r="H24" s="12">
         <v>200</v>

</xml_diff>

<commit_message>
update test cases for smart space
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CE953D-51E5-4267-B54D-0A3F6F6F21DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A684A3A-E4E3-481D-94F3-AA53967F1DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="676" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="676" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="751">
   <si>
     <t>description</t>
   </si>
@@ -8102,6 +8102,57 @@
 Point(type='Occupancy_Status',sourceId='')-&gt;Timeseries(captureTime)
 sourcesystem:iotgateway</t>
     </r>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Mode_Command_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_79692331.Present_Value",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Mode_Command_Update(input:
+   [
+        {
+          sourceId: "GmsDevice_1_7105_29360128.Present_Value",
+          value: "0"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+   Mode_Command_Update(input:
+   [
+        {
+          sourceId: "System1:GmsDevice_4_7130_29360128.Present_Value",
+          value: "1"
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
   </si>
 </sst>
 </file>
@@ -12046,8 +12097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2181B9E2-AEE2-4C11-98DD-ED06134DE024}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -13356,8 +13407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD40A695-640D-4069-93EC-24D7461E4F01}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -13442,7 +13493,7 @@
         <v>98</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>194</v>
+        <v>748</v>
       </c>
       <c r="E3" s="19">
         <v>200</v>
@@ -13471,7 +13522,7 @@
         <v>98</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>188</v>
+        <v>749</v>
       </c>
       <c r="E4" s="19">
         <v>200</v>
@@ -13500,7 +13551,7 @@
         <v>98</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>189</v>
+        <v>750</v>
       </c>
       <c r="E5" s="19">
         <v>200</v>

</xml_diff>

<commit_message>
update cases since the kg graph is changed
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E336324-69A1-49F8-9ECE-EF0AB6733620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EF4B8E-EB71-4793-89D8-98BD5BAAE6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="676" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="985">
   <si>
     <t>description</t>
   </si>
@@ -13144,6 +13144,75 @@
   <si>
     <t>SELECT dataLayerTime,co2 as Value,devEUI as PropertyId,sourceSystem from AM300_Data ad where devEUI = '24e124710b514794' 
 and dataLayerTime &gt;= $startTime AND dataLayerTime &lt;= $endTime order by dataLayerTime ASC</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_TRAINCONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_TRAINRESULT</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_PREDICTCONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_PREDICTRESULT</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_OPTIMALIZERESULT</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_OPTIMALIZECONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_SIMULATION</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_TOPOLOGY</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_OPTIMIZE_TARGET_TYPE</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_DASHBOARDCONFIG</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_METADATA</t>
+  </si>
+  <si>
+    <t>iems-config-CIMSOURCE_SECTIONALIZEDLINEARIZATION</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_TRAINCONFIG(cond:"",order:"") { createTime optimize_target_type_id simu_id train_cfg_ANN_YN train_cfg_LR_YN train_cfg_RFR_YN train_cfg_SVR_YN train_cfg_SmpEndTime train_cfg_SmpStTime train_cfg_Tree_YN train_cfg_aDa_YN train_cfg_obj_PT train_cfg_obligate1 train_cfg_obligate2 train_cfg_obligate3 train_cfg_obligate4 train_cfg_obligate5 train_cfg_obligate6 train_cfg_predict train_cfg_sample_PT train_cfg_time train_cfg_timetrg_YN}}</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_TRAINRESULT(cond:"",order:"") { variables train_result_obligate4 train_result_obligate5 train_result_obligate2 train_result_obligate3 optimize_target_type_id simu_id train_result_obligate1 config_id train_result_obligate6 runid }}</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_PREDICTRESULT(cond:"",order:"config_id ASC") { Predict_result_time Predict_result_aDa Predict_result_ANN optimize_target_type_id Predict_result_SP5 Predict_result_Tree Predict_result_LR Predict_result_SVR runid createTime variables predict_train_obj_wgt_defval Predict_result_obligate2 Predict_result_obligate1 Predict_result_RFR Predict_result_obligate6 simu_id Predict_result_obligate5 Predict_result_obligate4 Predict_result_obligate3 config_id Predict_result_AVG } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_OPTIMALIZECONFIG(cond:"",order:"") { isActive optimize_target_type_id optimalizeType opt_cfg_opt_starttime opt_cfg_user_def opt_pred_model opt_cfg_obligate3 rollTasksId opt_cfg_obligate2 opt_cfg_obligate5 createTime opt_cfg_obligate4 opt_cfg_obligate6 opt_cfg_emi_frac opt_name dash_cfg_id simu_id opt_cfg_opt_day opt_cfg_opt_frequency isRTCOP opt_cfg_cost_frac opt_methods rollType opt_cfg_obligate1 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_SIMULATION(cond:"",order:"") { updatatime historymap chartsetting createtime rtcountmap hiscountmap isTraining obligate1 obligate2 channels defcountmap user_id ispredict name obligate5 obligate6 treefile obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_TOPOLOGY(cond:"",order:"") { create_time topo_name simu_id obligate1 obligate2 topo_xml update_time update_user parent_id obligate5 obligate6 obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_OPTIMIZE_TARGET_TYPE(cond:"",order:"") { obligate1 obligate2 optimize_topo_selection optimize_type optimize_name obligate5 optimize_data_type obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_DASHBOARDCONFIG(cond:"",order:"") { dashparam name simu_id optimize_target_type_id } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_METADATA(cond:"",order:"") { obligate1 obligate2 name obligate5 params category obligate3 obligate4 } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_SECTIONALIZEDLINEARIZATION(cond:"",order:"") { tensor_index_counts target obligate1 obligate2 device_name model_name param obligate5 obligate3 obligate4 tensor_data } }</t>
+  </si>
+  <si>
+    <t>{CIMSOURCE_PREDICTCONFIG(cond:"",order:"") { predict_train_model createTime predict_train_obj_wgt_defval predict_cfg_obligate6 predict_cfg_obligate5 predict_cfg_obligate4 predict_cfg_obligate3 predict_cfg_obligate2 predict_cfg_obligate1 optimize_target_type_id simu_id predict_cfg_period predict_cfg_day predict_cfg_time } }</t>
   </si>
 </sst>
 </file>
@@ -13825,7 +13894,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -14058,78 +14127,246 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18"/>
+      <c r="A12" s="18" t="s">
+        <v>962</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>974</v>
+      </c>
+      <c r="D12" s="18">
+        <v>200</v>
+      </c>
+      <c r="E12" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18"/>
+      <c r="A13" s="18" t="s">
+        <v>963</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>975</v>
+      </c>
+      <c r="D13" s="18">
+        <v>200</v>
+      </c>
+      <c r="E13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18"/>
+      <c r="A14" s="18" t="s">
+        <v>964</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>984</v>
+      </c>
+      <c r="D14" s="18">
+        <v>200</v>
+      </c>
+      <c r="E14" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="18"/>
+      <c r="A15" s="18" t="s">
+        <v>965</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>976</v>
+      </c>
+      <c r="D15" s="18">
+        <v>200</v>
+      </c>
+      <c r="E15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="18"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="18"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="18"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="18"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="18"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>966</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>976</v>
+      </c>
+      <c r="D16" s="18">
+        <v>200</v>
+      </c>
+      <c r="E16" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>967</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>977</v>
+      </c>
+      <c r="D17" s="18">
+        <v>200</v>
+      </c>
+      <c r="E17" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>968</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>978</v>
+      </c>
+      <c r="D18" s="18">
+        <v>200</v>
+      </c>
+      <c r="E18" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>969</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>979</v>
+      </c>
+      <c r="D19" s="18">
+        <v>200</v>
+      </c>
+      <c r="E19" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>970</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>980</v>
+      </c>
+      <c r="D20" s="18">
+        <v>200</v>
+      </c>
+      <c r="E20" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>971</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>981</v>
+      </c>
+      <c r="D21" s="18">
+        <v>200</v>
+      </c>
+      <c r="E21" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>972</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>982</v>
+      </c>
+      <c r="D22" s="18">
+        <v>200</v>
+      </c>
+      <c r="E22" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>973</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>983</v>
+      </c>
+      <c r="D23" s="18">
+        <v>200</v>
+      </c>
+      <c r="E23" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>

</xml_diff>

<commit_message>
update iems-api-engine-test-data.xlsx and iems-connector-test-data.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EF4B8E-EB71-4793-89D8-98BD5BAAE6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AD07F6-7956-4AE2-A7EA-441CB2156B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="676" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13891,15 +13891,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A24" sqref="A24:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="54.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="60.6640625" style="6" customWidth="1"/>
     <col min="4" max="6" width="12.6640625" style="1" customWidth="1"/>
@@ -14365,12 +14365,6 @@
       <c r="F23" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>